<commit_message>
copy changes, most cost effective sld
</commit_message>
<xml_diff>
--- a/src/data/capex.xlsx
+++ b/src/data/capex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fotheringhamr\Documents\Python Scripts\another_capex\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E01FA47-FA30-4D2C-AD8E-D7B7855EC516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EDB562-61D3-444A-8E3D-C440053ED5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5640" windowWidth="29040" windowHeight="15720" xr2:uid="{0D85ABAC-D8F4-4B38-A0CB-19C39BE76A6F}"/>
+    <workbookView xWindow="-18315" yWindow="-2385" windowWidth="17250" windowHeight="11565" xr2:uid="{0D85ABAC-D8F4-4B38-A0CB-19C39BE76A6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Capex: Array</t>
-  </si>
   <si>
     <t>Capex: Transmission Cable</t>
   </si>
@@ -85,6 +82,9 @@
   <si>
     <t>Availability: Onshore Transformers</t>
   </si>
+  <si>
+    <t>Capex: Midpoint Sub</t>
+  </si>
 </sst>
 </file>
 
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -326,7 +326,6 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,61 +663,61 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:21" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="25"/>
+      <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>

</xml_diff>